<commit_message>
add SRS and Imapct analysis reviews
</commit_message>
<xml_diff>
--- a/Monitor and Control/Car-Reviews.xlsx
+++ b/Monitor and Control/Car-Reviews.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aml\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\QA\QA_project\Car-Bookings\Monitor and Control\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PMP" sheetId="1" r:id="rId1"/>
     <sheet name="SRS" sheetId="2" r:id="rId2"/>
     <sheet name="Design" sheetId="3" r:id="rId3"/>
     <sheet name="Coding" sheetId="4" r:id="rId4"/>
-    <sheet name="Progress" sheetId="5" r:id="rId5"/>
-    <sheet name="Option" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="Immapc Analysis" sheetId="7" r:id="rId5"/>
+    <sheet name="Progress" sheetId="5" r:id="rId6"/>
+    <sheet name="Option" sheetId="6" state="hidden" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Coding!$A$2:$H$15</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="135">
   <si>
     <t>Version No.</t>
   </si>
@@ -399,6 +400,61 @@
   <si>
     <t>Upated CM section to clarify the release version on GitHub (Vx)</t>
   </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>Eng Amr</t>
+  </si>
+  <si>
+    <t>14-5-2022</t>
+  </si>
+  <si>
+    <t>In changing the project manager impact analysis table in actions column divide actions under time,cost or project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aml </t>
+  </si>
+  <si>
+    <t>17-5-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In changing the project manager impact analysis table in impact column first point be more specific in the extra time that will be needed as an impact on project manager change </t>
+  </si>
+  <si>
+    <t>V1.1</t>
+  </si>
+  <si>
+    <t>In time pressure impact analysis table in actions column divide actions under time,cost or project</t>
+  </si>
+  <si>
+    <t>19-5-2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In removing add admin and add users features impact analysis table (change_003) the impact on cost is not clear
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In removing add admin and add users features impact analysis table (change_003) the different actions that can be taken is not clear and need modification according to team discussions </t>
+  </si>
+  <si>
+    <t>Basma Galal</t>
+  </si>
+  <si>
+    <t>Aya Tarek</t>
+  </si>
+  <si>
+    <t>In removing add admin and add users features impact analysis table (change_003) the chosen actions should be changed according to the updates of the actions that have been discussed with the team</t>
+  </si>
+  <si>
+    <t>18-5-2022</t>
+  </si>
+  <si>
+    <t>Change update feature ( CR-006) desription to reflect the changes</t>
+  </si>
+  <si>
+    <t>Identify priority measurement (High - Medium-Low)</t>
+  </si>
 </sst>
 </file>
 
@@ -468,7 +524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -687,11 +743,89 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -783,6 +917,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -791,11 +937,139 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="64">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA8D08D"/>
+          <bgColor rgb="FFA8D08D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF7CAAC"/>
+          <bgColor rgb="FFF7CAAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FFD8D8D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA8D08D"/>
+          <bgColor rgb="FFA8D08D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF7CAAC"/>
+          <bgColor rgb="FFF7CAAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FFD8D8D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFA8D08D"/>
+          <bgColor rgb="FFA8D08D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF7CAAC"/>
+          <bgColor rgb="FFF7CAAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD8D8D8"/>
+          <bgColor rgb="FFD8D8D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1588,7 +1862,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3084,16 +3358,16 @@
       <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="72.5546875" customWidth="1"/>
-    <col min="6" max="7" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="72.5703125" customWidth="1"/>
+    <col min="6" max="7" width="13.85546875" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="10" width="8.6640625" customWidth="1"/>
+    <col min="9" max="10" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.5" customHeight="1">
@@ -7701,42 +7975,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F19 F21:F1000">
-    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F19 F21:F1000">
-    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F19 F21:F1000">
-    <cfRule type="cellIs" dxfId="49" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F19 F21:F1000">
-    <cfRule type="cellIs" dxfId="48" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7761,22 +8035,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="70.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="27" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="70.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="27" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="25.5" customHeight="1">
@@ -8263,10 +8537,10 @@
       <c r="C20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="46">
         <v>44692</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="47" t="s">
         <v>60</v>
       </c>
       <c r="F20" s="14" t="s">
@@ -8275,17 +8549,61 @@
       <c r="G20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="46">
         <v>44694</v>
       </c>
     </row>
     <row r="21" spans="1:27" ht="14.25" customHeight="1">
-      <c r="F21" s="11"/>
-      <c r="H21" s="12"/>
-    </row>
-    <row r="22" spans="1:27" ht="14.25" customHeight="1">
-      <c r="F22" s="11"/>
-      <c r="H22" s="12"/>
+      <c r="A21" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="52">
+        <v>44695</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="51">
+        <v>44698</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" s="44" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A22" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="52">
+        <v>44695</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="51">
+        <v>44698</v>
+      </c>
     </row>
     <row r="23" spans="1:27" ht="14.25" customHeight="1">
       <c r="F23" s="11"/>
@@ -11421,43 +11739,63 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H1"/>
-  <conditionalFormatting sqref="F1:F17 F19:F1000">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
+  <conditionalFormatting sqref="F1:F17 F23:F1000 F19:F21">
+    <cfRule type="cellIs" dxfId="55" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F17 F19:F1000">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+  <conditionalFormatting sqref="F1:F17 F23:F1000 F19:F21">
+    <cfRule type="cellIs" dxfId="54" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F17 F19:F1000">
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
+  <conditionalFormatting sqref="F1:F17 F23:F1000 F19:F21">
+    <cfRule type="cellIs" dxfId="53" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F17 F19:F1000">
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
+  <conditionalFormatting sqref="F1:F17 F23:F1000 F19:F21">
+    <cfRule type="cellIs" dxfId="52" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="42" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="14" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="41" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="15" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="40" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="16" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11485,18 +11823,18 @@
   </sheetPr>
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="55.109375" customWidth="1"/>
-    <col min="6" max="25" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="55.140625" customWidth="1"/>
+    <col min="6" max="25" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="25.5" customHeight="1">
@@ -11587,7 +11925,7 @@
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
     </row>
-    <row r="3" spans="1:26" ht="14.4">
+    <row r="3" spans="1:26">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -11835,7 +12173,7 @@
       <c r="Y8" s="5"/>
       <c r="Z8" s="5"/>
     </row>
-    <row r="9" spans="1:26" thickBot="1">
+    <row r="9" spans="1:26" ht="15.75" thickBot="1">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -12091,7 +12429,7 @@
         <v>44695</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.4">
+    <row r="16" spans="1:26">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -12119,7 +12457,7 @@
       <c r="Y16" s="5"/>
       <c r="Z16" s="5"/>
     </row>
-    <row r="17" spans="1:26" ht="14.4">
+    <row r="17" spans="1:26">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -39589,122 +39927,122 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F7 F16:F997">
-    <cfRule type="cellIs" dxfId="39" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="21" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F7 F16:F997">
-    <cfRule type="cellIs" dxfId="38" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="22" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F7 F16:F997">
-    <cfRule type="cellIs" dxfId="37" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="23" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F7 F16:F997">
-    <cfRule type="cellIs" dxfId="36" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="24" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="35" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="17" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="34" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="18" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="33" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="19" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="32" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="20" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F10">
-    <cfRule type="cellIs" dxfId="31" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="13" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F10">
-    <cfRule type="cellIs" dxfId="30" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="14" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F10">
-    <cfRule type="cellIs" dxfId="29" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="15" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F10">
-    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="16" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="26" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F13">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F13">
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F13">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12:F13">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F15">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F15">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F15">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14:F15">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39733,20 +40071,20 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="53.44140625" customWidth="1"/>
-    <col min="6" max="6" width="27.109375" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="53.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="9" width="27.109375" customWidth="1"/>
-    <col min="10" max="26" width="8.6640625" customWidth="1"/>
+    <col min="8" max="9" width="27.140625" customWidth="1"/>
+    <col min="10" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="20.399999999999999" customHeight="1" thickBot="1">
+    <row r="1" spans="1:26" ht="20.45" customHeight="1" thickBot="1">
       <c r="A1" s="29" t="s">
         <v>101</v>
       </c>
@@ -41332,62 +41670,62 @@
   </sheetData>
   <autoFilter ref="A2:H15"/>
   <conditionalFormatting sqref="F2:F3 F13:F16 F5:F10">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F3 F13:F16 F5:F10">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F3 F13:F16 F5:F10">
-    <cfRule type="cellIs" dxfId="13" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F3 F13:F16 F5:F10">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"Need Approval"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41410,19 +41748,417 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="25.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+    </row>
+    <row r="2" spans="1:26" ht="75">
+      <c r="A2" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="120">
+      <c r="A3" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="75">
+      <c r="A4" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
+    </row>
+    <row r="6" spans="1:26" ht="90">
+      <c r="A6" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="135">
+      <c r="A7" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="135">
+      <c r="A8" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="33"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:H5"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F1">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"Need Approval"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>"Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="12" width="8.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" customWidth="1"/>
-    <col min="14" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.25" customHeight="1">
@@ -41452,7 +42188,7 @@
       <c r="X1" s="27"/>
     </row>
     <row r="2" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="37" t="s">
         <v>93</v>
       </c>
       <c r="B2" s="28" t="s">
@@ -41470,7 +42206,7 @@
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="37" t="s">
         <v>94</v>
       </c>
       <c r="M2" s="28" t="s">
@@ -41492,7 +42228,7 @@
       <c r="X2" s="27"/>
     </row>
     <row r="3" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A3" s="34"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="28" t="s">
         <v>12</v>
       </c>
@@ -41508,13 +42244,13 @@
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
       <c r="K3" s="27"/>
-      <c r="L3" s="34"/>
+      <c r="L3" s="38"/>
       <c r="M3" s="28" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="28">
         <f>COUNTIFS(SRS!F:F,"Closed")</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O3" s="27"/>
       <c r="P3" s="27"/>
@@ -41528,7 +42264,7 @@
       <c r="X3" s="27"/>
     </row>
     <row r="4" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A4" s="34"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="28" t="s">
         <v>95</v>
       </c>
@@ -41544,7 +42280,7 @@
       <c r="I4" s="27"/>
       <c r="J4" s="27"/>
       <c r="K4" s="27"/>
-      <c r="L4" s="34"/>
+      <c r="L4" s="38"/>
       <c r="M4" s="28" t="s">
         <v>95</v>
       </c>
@@ -41564,7 +42300,7 @@
       <c r="X4" s="27"/>
     </row>
     <row r="5" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A5" s="34"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="28" t="s">
         <v>96</v>
       </c>
@@ -41580,7 +42316,7 @@
       <c r="I5" s="27"/>
       <c r="J5" s="27"/>
       <c r="K5" s="27"/>
-      <c r="L5" s="34"/>
+      <c r="L5" s="38"/>
       <c r="M5" s="28" t="s">
         <v>96</v>
       </c>
@@ -41600,7 +42336,7 @@
       <c r="X5" s="27"/>
     </row>
     <row r="6" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A6" s="35"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="28" t="s">
         <v>97</v>
       </c>
@@ -41616,13 +42352,13 @@
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
       <c r="K6" s="27"/>
-      <c r="L6" s="35"/>
+      <c r="L6" s="39"/>
       <c r="M6" s="28" t="s">
         <v>97</v>
       </c>
       <c r="N6" s="28">
         <f>SUM(N2:N5)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O6" s="27"/>
       <c r="P6" s="27"/>
@@ -42026,7 +42762,7 @@
       <c r="X21" s="27"/>
     </row>
     <row r="22" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="37" t="s">
         <v>98</v>
       </c>
       <c r="B22" s="28" t="s">
@@ -42044,7 +42780,7 @@
       <c r="I22" s="27"/>
       <c r="J22" s="27"/>
       <c r="K22" s="27"/>
-      <c r="L22" s="36" t="s">
+      <c r="L22" s="40" t="s">
         <v>111</v>
       </c>
       <c r="M22" s="28" t="s">
@@ -42066,7 +42802,7 @@
       <c r="X22" s="27"/>
     </row>
     <row r="23" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A23" s="34"/>
+      <c r="A23" s="38"/>
       <c r="B23" s="28" t="s">
         <v>12</v>
       </c>
@@ -42082,7 +42818,7 @@
       <c r="I23" s="27"/>
       <c r="J23" s="27"/>
       <c r="K23" s="27"/>
-      <c r="L23" s="34"/>
+      <c r="L23" s="38"/>
       <c r="M23" s="28" t="s">
         <v>12</v>
       </c>
@@ -42102,7 +42838,7 @@
       <c r="X23" s="27"/>
     </row>
     <row r="24" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A24" s="34"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="28" t="s">
         <v>95</v>
       </c>
@@ -42118,7 +42854,7 @@
       <c r="I24" s="27"/>
       <c r="J24" s="27"/>
       <c r="K24" s="27"/>
-      <c r="L24" s="34"/>
+      <c r="L24" s="38"/>
       <c r="M24" s="28" t="s">
         <v>95</v>
       </c>
@@ -42138,7 +42874,7 @@
       <c r="X24" s="27"/>
     </row>
     <row r="25" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A25" s="34"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="28" t="s">
         <v>96</v>
       </c>
@@ -42154,7 +42890,7 @@
       <c r="I25" s="27"/>
       <c r="J25" s="27"/>
       <c r="K25" s="27"/>
-      <c r="L25" s="34"/>
+      <c r="L25" s="38"/>
       <c r="M25" s="28" t="s">
         <v>96</v>
       </c>
@@ -42174,7 +42910,7 @@
       <c r="X25" s="27"/>
     </row>
     <row r="26" spans="1:24" ht="14.25" customHeight="1">
-      <c r="A26" s="35"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="28" t="s">
         <v>97</v>
       </c>
@@ -42190,7 +42926,7 @@
       <c r="I26" s="27"/>
       <c r="J26" s="27"/>
       <c r="K26" s="27"/>
-      <c r="L26" s="35"/>
+      <c r="L26" s="39"/>
       <c r="M26" s="28" t="s">
         <v>97</v>
       </c>
@@ -45696,17 +46432,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="14.25" customHeight="1">

</xml_diff>